<commit_message>
training weights in progress
</commit_message>
<xml_diff>
--- a/eval_results.xlsx
+++ b/eval_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haoran/Documents/thesis_schema_integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492C1311-5A55-224C-A097-CA9F82FE6C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E413129A-D1C8-D243-839B-1C2447132064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="3200" windowWidth="35700" windowHeight="18340" xr2:uid="{07961CF2-8B35-3E4A-A201-E2C4464309B0}"/>
   </bookViews>
@@ -267,18 +267,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -292,6 +280,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,7 +652,7 @@
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -664,10 +664,10 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -676,7 +676,7 @@
       <c r="D3">
         <v>0.09</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <v>0.28570000000000001</v>
       </c>
       <c r="F3" s="6">
@@ -685,19 +685,19 @@
       <c r="G3" s="5">
         <v>0.2</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="13">
         <v>0.21879999999999999</v>
       </c>
       <c r="I3" s="6"/>
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>0.39129999999999998</v>
       </c>
       <c r="E4" s="6">
@@ -706,33 +706,33 @@
       <c r="F4" s="6">
         <v>0.13039999999999999</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="9">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="13">
         <v>0.30430000000000001</v>
       </c>
       <c r="I4" s="6"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>0.36249999999999999</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="13">
         <v>0.28570000000000001</v>
       </c>
       <c r="F5" s="6">
         <v>0.2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="9">
         <v>0.2</v>
       </c>
       <c r="H5" s="6">
@@ -742,12 +742,12 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>0.42030000000000001</v>
       </c>
       <c r="E6" s="6">
@@ -756,18 +756,18 @@
       <c r="F6" s="6">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="9">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="13">
         <v>0.36230000000000001</v>
       </c>
       <c r="I6" s="6"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -776,28 +776,28 @@
       <c r="D7" s="6">
         <v>0.23949999999999999</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="13">
         <v>0.28570000000000001</v>
       </c>
       <c r="F7" s="6">
         <v>0.1764</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="9">
         <v>0.1764</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <v>0.5</v>
       </c>
       <c r="I7" s="6"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>0.46929999999999999</v>
       </c>
       <c r="E8" s="6">
@@ -806,64 +806,64 @@
       <c r="F8" s="6">
         <v>3.0599999999999999E-2</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="13">
         <v>0.28570000000000001</v>
       </c>
       <c r="I8" s="6"/>
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="8">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="8">
         <v>0</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>0.1764</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="9">
         <v>0.1764</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="8">
         <v>3.44E-2</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="13">
         <v>4.2099999999999999E-2</v>
       </c>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="12">
         <v>0.6956</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="8">
         <v>0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="8">
         <v>0.13039999999999999</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="9">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>0.52170000000000005</v>
       </c>
       <c r="I10" s="6">
@@ -872,26 +872,26 @@
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="8">
         <v>8.9599999999999999E-2</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <v>0.18179999999999999</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="8">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="9">
         <v>0.16669999999999999</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="12">
         <v>0.2064</v>
       </c>
       <c r="I11" s="6">
@@ -900,24 +900,24 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="12">
         <v>0.59</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="8">
         <v>0.02</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="8">
         <v>0.03</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="9">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>0.45</v>
       </c>
       <c r="I12" s="6">
@@ -926,52 +926,52 @@
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="8">
         <v>0.17330000000000001</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="8">
         <v>0.15379999999999999</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="8">
         <v>0.16669999999999999</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="10">
         <v>0.16669999999999999</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="12">
         <v>0.46889999999999998</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="13">
         <v>0.2059</v>
       </c>
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="8">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="8">
         <v>1.37E-2</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="10">
         <v>0.13039999999999999</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="14">
         <v>0.38069999999999998</v>
       </c>
       <c r="I14" s="6">
@@ -1027,182 +1027,182 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -1273,192 +1273,192 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="11"/>
+      <c r="C38" s="16">
+        <v>17</v>
+      </c>
+      <c r="D38" s="16">
+        <v>7</v>
+      </c>
+      <c r="E38" s="16">
+        <v>15</v>
+      </c>
+      <c r="F38" s="16">
+        <v>6</v>
+      </c>
+      <c r="G38" s="15"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="11"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="15"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="11"/>
+      <c r="C40" s="16">
+        <v>14.67</v>
+      </c>
+      <c r="D40" s="16">
+        <v>2.33</v>
+      </c>
+      <c r="E40" s="16">
+        <v>5</v>
+      </c>
+      <c r="F40" s="16">
+        <v>13</v>
+      </c>
+      <c r="G40" s="15"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="11"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="15"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="11"/>
+      <c r="C42" s="16">
+        <v>26.4</v>
+      </c>
+      <c r="D42" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="E42" s="16">
+        <v>3.4</v>
+      </c>
+      <c r="F42" s="16">
+        <v>8</v>
+      </c>
+      <c r="G42" s="15"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="11"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
+      <c r="C44" s="17">
+        <v>63</v>
+      </c>
+      <c r="D44" s="17">
+        <v>0</v>
+      </c>
+      <c r="E44" s="17">
+        <v>17</v>
+      </c>
+      <c r="F44" s="17">
+        <v>29</v>
+      </c>
+      <c r="G44" s="17">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
+      <c r="C46" s="17">
+        <v>70.2</v>
+      </c>
+      <c r="D46" s="17">
+        <v>2</v>
+      </c>
+      <c r="E46" s="17">
+        <v>3.6</v>
+      </c>
+      <c r="F46" s="17">
+        <v>16.2</v>
+      </c>
+      <c r="G46" s="17">
+        <v>20.399999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10" t="s">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
+      <c r="C48" s="17">
+        <v>65</v>
+      </c>
+      <c r="D48" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="E48" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="F48" s="17">
+        <v>13.9</v>
+      </c>
+      <c r="G48" s="17">
+        <v>16.5</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="G23:G24"/>
@@ -1475,13 +1475,67 @@
     <mergeCell ref="A25:A30"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G46:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>